<commit_message>
modified:   README.md         new file:   deepseek/README.md         new file:   llm-fastapi/README.md         new file:   llm-summarize-document/README.md         modified:   llm-summarize-document/llm_summarize_document.py         modified:   llm-summarize-document/output_rag/langchain_demo_rag_answer.txt         modified:   llm-summarize-document/output_rag/sample_rag_answer.txt         modified:   llm-summarize-document/output_rag/summaries.xlsx         new file:   streamlit/README.md
</commit_message>
<xml_diff>
--- a/llm-summarize-document/output_rag/summaries.xlsx
+++ b/llm-summarize-document/output_rag/summaries.xlsx
@@ -453,7 +453,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>LangChain is a framework simplifying the creation of LLM-based applications by offering modular components, data integration capabilities, and agent frameworks. It's designed for use cases like chatbots, question answering systems, and various text generation tasks, supported by comprehensive documentation and resources available from the LangChain team and Brandon Hancock’s YouTube channel.</t>
+          <t>LangChain is a framework designed to simplify the building of LLM-powered applications. Its key features involve modular components, seamless data integration, agent frameworks, memory management, prompt engineering, and chain optimization, enabling a wide range of applications like chatbots, question answering systems, and text generation tools. Resources like documentation and a YouTube channel by Brandon Hancock are available for further learning.</t>
         </is>
       </c>
     </row>
@@ -465,7 +465,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>This document is a placeholder text – “Lorem Ipsum” – commonly used in graphic design and publishing as a dummy text to demonstrate the visual form of a document or typeface without conveying specific meaning.</t>
+          <t>This document is a placeholder text (Lorem Ipsum) – a standard dummy text used in design and printing to demonstrate the visual form of a document without relying on meaningful content.</t>
         </is>
       </c>
     </row>

</xml_diff>